<commit_message>
Added more gerber outputs, updated BOM, changed PCB, and added Arduino code to generate a fixed PWM as a test.
</commit_message>
<xml_diff>
--- a/Schematic_Artifacts/PSU4PSU.xlsx
+++ b/Schematic_Artifacts/PSU4PSU.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AridDay\Desktop\PSU4PSU\Schematic_Artifacts\Project Outputs for PSU4PSU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AridDay\Desktop\PSU4PSU\Schematic_Artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1329AC55-97AD-4E87-BDB1-DA2130C08CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8016C32-E4F4-4BBB-A309-71321F65CA05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{329F267F-12D1-4CDB-AC34-15097280C5CC}"/>
+    <workbookView xWindow="-28920" yWindow="2385" windowWidth="29040" windowHeight="15720" xr2:uid="{329F267F-12D1-4CDB-AC34-15097280C5CC}"/>
   </bookViews>
   <sheets>
     <sheet name="PSU4PSU" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="105">
   <si>
     <t>Line #</t>
   </si>
@@ -351,6 +351,9 @@
   </si>
   <si>
     <t>CRCW080520K0FKTA</t>
+  </si>
+  <si>
+    <t>Resistor (750 ohm)</t>
   </si>
 </sst>
 </file>
@@ -730,7 +733,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1209,7 +1212,7 @@
         <v>65</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>66</v>
+        <v>104</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>67</v>

</xml_diff>